<commit_message>
site 2 3 done
</commit_message>
<xml_diff>
--- a/files/input.xlsx
+++ b/files/input.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Link 1</t>
   </si>
@@ -32,24 +32,6 @@
   </si>
   <si>
     <t>https://www.casa.it/srp/?tr=vendita&amp;exclude_auction=true&amp;sortType=surface_asc&amp;geopolygon={%22polygon%22:[[43.55615623790824%2C10.312495672887065]%2C[43.55635061711003%2C10.312699520772197]%2C[43.559367301940625%2C10.314759457295635]%2C[43.55970939068563%2C10.314501965230205]%2C[43.558418772988844%2C10.30888005513499]%2C[43.5575635291655%2C10.309169733708599]%2C[43.557097027418095%2C10.309470141118267]%2C[43.557097027418095%2C10.310060227101543]%2C[43.556109586806535%2C10.310489380543926]]%2C%22bbox%22:[[43.56155197165589%2C10.30314012784312]%2C[43.55426683939984%2C10.320499384587505]]%2C%22zoom%22:17}&amp;precision=7&amp;propertyTypeGroup=case</t>
-  </si>
-  <si>
-    <t>https://www.immobiliare.it/search-list/?vrt=43.547918%2C10.309693%3B43.548431%2C10.309693%3B43.548626%2C10.304639%3B43.547926%2C10.304468%3B43.547179%2C10.304414%3B43.547498%2C10.306882%3B43.547397%2C10.309414%3B43.547156%2C10.310615%3B43.547319%2C10.311152%3B43.547701%2C10.311087%3B43.547879%2C10.310165%3B43.547918%2C10.309693&amp;idContratto=1&amp;idCategoria=1&amp;tipoProprieta=1&amp;criterio=superficie&amp;ordine=asc&amp;noAste=1&amp;__lang=it&amp;pag=1&amp;slau=1</t>
-  </si>
-  <si>
-    <t>https://www.idealista.it/aree/vendita-case/con-aste_no/?ordine=area-asc&amp;shape=%28%28_ixhGqq%7B%7D%40eHg%40PaED%7DFJuCBgDHeG%7EADf%40_EIgAvAe%40d%40jCMLc%40lFQzMz%40nN%29%29</t>
-  </si>
-  <si>
-    <t>https://www.casa.it/srp/?page=2&amp;tr=vendita&amp;exclude_auction=true&amp;sortType=surface_asc&amp;geopolygon={%22polygon%22:[[43.55615623790824,10.312495672887065],[43.55635061711003,10.312699520772197],[43.559367301940625,10.314759457295635],[43.55970939068563,10.314501965230205],[43.558418772988844,10.30888005513499],[43.5575635291655,10.309169733708599],[43.557097027418095,10.309470141118267],[43.557097027418095,10.310060227101543],[43.556109586806535,10.310489380543926]],%22bbox%22:[[43.56155197165589,10.30314012784312],[43.55426683939984,10.320499384587505]],%22zoom%22:17}&amp;precision=7&amp;propertyTypeGroup=case</t>
-  </si>
-  <si>
-    <t>https://www.immobiliare.it/search-list/?vrt=43.548533%2C10.317353%3B43.549948%2C10.315754%3B43.549645%2C10.315132%3B43.550539%2C10.31422%3B43.549792%2C10.313222%3B43.548019%2C10.311999%3B43.547662%2C10.312171%3B43.547032%2C10.312557%3B43.547265%2C10.313255%3B43.547211%2C10.313491%3B43.547351%2C10.313512%3B43.548533%2C10.317353&amp;idContratto=1&amp;idCategoria=1&amp;tipoProprieta=1&amp;criterio=superficie&amp;ordine=asc&amp;noAste=1&amp;__lang=it&amp;pag=1</t>
-  </si>
-  <si>
-    <t>https://www.idealista.it/aree/vendita-case/con-aste_no/?ordine=area-asc&amp;shape=%28%28_nxhGca%7D%7D%40cGsCaDsC%7BAeCtBmCcAaBtIiKvH%7C%5C%7DDhB%29%29</t>
-  </si>
-  <si>
-    <t>https://www.casa.it/srp/?page=3&amp;tr=vendita&amp;exclude_auction=true&amp;sortType=surface_asc&amp;geopolygon={%22polygon%22:[[43.55615623790824,10.312495672887065],[43.55635061711003,10.312699520772197],[43.559367301940625,10.314759457295635],[43.55970939068563,10.314501965230205],[43.558418772988844,10.30888005513499],[43.5575635291655,10.309169733708599],[43.557097027418095,10.309470141118267],[43.557097027418095,10.310060227101543],[43.556109586806535,10.310489380543926]],%22bbox%22:[[43.56155197165589,10.30314012784312],[43.55426683939984,10.320499384587505]],%22zoom%22:17}&amp;precision=7&amp;propertyTypeGroup=case</t>
   </si>
 </sst>
 </file>
@@ -447,7 +429,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -480,28 +462,6 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>